<commit_message>
Hussain Wali Audio 260 sentences
</commit_message>
<xml_diff>
--- a/burushaski sentences.xlsx
+++ b/burushaski sentences.xlsx
@@ -15,192 +15,375 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="376">
-  <si>
-    <t>vae thamene paisa ayidimi</t>
-  </si>
-  <si>
-    <t>vae te yarbullhtuk paisa ayidimi</t>
-  </si>
-  <si>
-    <t>ve yaarbullhtuk paisa ayidimi</t>
-  </si>
-  <si>
-    <t>ve gucxattinga paisa ayidimi</t>
-  </si>
-  <si>
-    <t>ve shama paisa ayidimi</t>
-  </si>
-  <si>
-    <t>ve saattik paisa ayidimi</t>
-  </si>
-  <si>
-    <t>ve hekan paisa ayidimi</t>
-  </si>
-  <si>
-    <t>ve butt paisa ayidimi</t>
-  </si>
-  <si>
-    <t>ve fukan paisa ayidimi</t>
-  </si>
-  <si>
-    <t>ve kaman paisa ayidimi</t>
-  </si>
-  <si>
-    <t>ve ajo paisa ayidimi</t>
-  </si>
-  <si>
-    <t>ve angaro omoos ayidimi</t>
-  </si>
-  <si>
-    <t>ve ccandurare omoos ayidimi</t>
-  </si>
-  <si>
-    <t>ve buddu omoos ayidimi</t>
-  </si>
-  <si>
-    <t>ve berespate omoos ayidimi</t>
-  </si>
-  <si>
-    <t>ve addite omoos ayidimi</t>
-  </si>
-  <si>
-    <t>ve shumshere omoos ayidimi</t>
-  </si>
-  <si>
-    <t>ve shukuru omoos ayidimi</t>
-  </si>
-  <si>
-    <t>ve taene omoos ayidimi</t>
-  </si>
-  <si>
-    <t>ve thamene omoos ayidimi</t>
-  </si>
-  <si>
-    <t>ve teyarbullhtuk omoos ayidimi</t>
-  </si>
-  <si>
-    <t>ve yaarbullhtuk omoos ayidimi</t>
-  </si>
-  <si>
-    <t>ve gucxattinga omoos ayidimi</t>
-  </si>
-  <si>
-    <t>ve shama omoos ayidimi</t>
-  </si>
-  <si>
-    <t>ve saattik omoos ayidimi</t>
-  </si>
-  <si>
-    <t>ve hekan omoos ayidimi</t>
-  </si>
-  <si>
-    <t>ve butt omoos ayidimi</t>
-  </si>
-  <si>
-    <t>ve fukan omoos ayidimi</t>
-  </si>
-  <si>
-    <t>ve kaman omoos ayidimi</t>
-  </si>
-  <si>
-    <t>ve ajo omoos ayidimi</t>
-  </si>
-  <si>
-    <t>ne angaro mos ayidimi</t>
-  </si>
-  <si>
-    <t>ne ccandurare moos ayidimi</t>
-  </si>
-  <si>
-    <t>ne buddu moos ayidimi</t>
-  </si>
-  <si>
-    <t>ne berespate moos ayidimi</t>
-  </si>
-  <si>
-    <t>ne addite moos ayidimi</t>
-  </si>
-  <si>
-    <t>ne shumshere moos ayidimi</t>
-  </si>
-  <si>
-    <t>ne shukuru moos ayidimi</t>
-  </si>
-  <si>
-    <t>ne taene moos ayidimi</t>
-  </si>
-  <si>
-    <t>ne thamene moos ayidimi</t>
-  </si>
-  <si>
-    <t>ne teyarbullhtuk moos ayidimi</t>
-  </si>
-  <si>
-    <t>ne yaarbullhtuk moos ayidimi</t>
-  </si>
-  <si>
-    <t>ne gucxattinga moos ayidimi</t>
-  </si>
-  <si>
-    <t>ne shama moos ayidimi</t>
-  </si>
-  <si>
-    <t>ne saattik moos ayidimi</t>
-  </si>
-  <si>
-    <t>ne hekan moos ayidimi</t>
-  </si>
-  <si>
-    <t>ne butt moos ayidimi</t>
-  </si>
-  <si>
-    <t>ne fukan moos ayidimi</t>
-  </si>
-  <si>
-    <t>ne kaman moos ayidimi</t>
-  </si>
-  <si>
-    <t>ne ajo moos ayidimi</t>
-  </si>
-  <si>
-    <t>salam lala</t>
-  </si>
-  <si>
-    <t>ja jee she be, acxhan api</t>
-  </si>
-  <si>
-    <t>Ja durdana cchel phat nety mel bota meyamba</t>
-  </si>
-  <si>
-    <t>Acxhan mani ka yasin a ccheran</t>
-  </si>
-  <si>
-    <t>xakun a baspur shei</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="418">
+  <si>
+    <t>bo zali ba ?</t>
+  </si>
+  <si>
+    <t>akhuing ajo shua gunz an dua gute shahar ka ajo shua shahar an dua</t>
+  </si>
+  <si>
+    <t>paqo sxhe</t>
+  </si>
+  <si>
+    <t>cchel mene</t>
+  </si>
+  <si>
+    <t>ja gamburi akkhosh</t>
+  </si>
+  <si>
+    <t>ja guliab gamburi akkhosh</t>
+  </si>
+  <si>
+    <t>ja cchella qaq amanamba</t>
+  </si>
+  <si>
+    <t>un guwarumba</t>
+  </si>
+  <si>
+    <t>un sxheli guwanumba</t>
+  </si>
+  <si>
+    <t>ne giraashumbai</t>
+  </si>
+  <si>
+    <t>ne girminchumbai</t>
+  </si>
+  <si>
+    <t>nae giraashumbai</t>
+  </si>
+  <si>
+    <t>nae girminchumbai</t>
+  </si>
+  <si>
+    <t>ayash gulabi isxhqam manumbi akhuing</t>
+  </si>
+  <si>
+    <t>paqo sxhe dan ayi sxhe</t>
+  </si>
+  <si>
+    <t>Le halles sena go bo doro dua</t>
+  </si>
+  <si>
+    <t>ja ka un neme te doro net cchuren</t>
+  </si>
+  <si>
+    <t>jaa acce bo bika gogga gucham</t>
+  </si>
+  <si>
+    <t>jaacce bo api</t>
+  </si>
+  <si>
+    <t>jaa acce bi</t>
+  </si>
+  <si>
+    <t>jaacce bi</t>
+  </si>
+  <si>
+    <t>ja sattik khela neyamam ajo maza diya jagga ne nnyu halles ajo wali</t>
+  </si>
+  <si>
+    <t>ja gogga han baran siyama agar ggafa akuwayumba ka</t>
+  </si>
+  <si>
+    <t>un ajo gukhar thathall ayet bae ka</t>
+  </si>
+  <si>
+    <t>Javaayu 100 ggaring har jawaane etas dua le akhuyng shaam khasxh</t>
+  </si>
+  <si>
+    <t>Bess aye sxhe chhap she</t>
+  </si>
+  <si>
+    <t>ne sheghetan mull cce dis na darhkut bull cce dis</t>
+  </si>
+  <si>
+    <t>ge aye sheng naa</t>
+  </si>
+  <si>
+    <t>jaa acce thosxh mobile an bim</t>
+  </si>
+  <si>
+    <t>Ayar yatte dapherhkan nawall cxoqaa amana</t>
+  </si>
+  <si>
+    <t>tayillcc bathanan manisxh bulyainge baraan manisxh</t>
+  </si>
+  <si>
+    <t>Jawayu akhuyng shaam khasxh berum echa llayuman ka girminas dua te yate ja echam</t>
+  </si>
+  <si>
+    <t>ajo chhap api</t>
+  </si>
+  <si>
+    <t>mo mucxhan api</t>
+  </si>
+  <si>
+    <t>jaa acxhan api</t>
+  </si>
+  <si>
+    <t>vae ucxhan api</t>
+  </si>
+  <si>
+    <t>vae shaama paisa ayideemi</t>
+  </si>
+  <si>
+    <t>vae taene omoos ayideemi</t>
+  </si>
+  <si>
+    <t>vae thamene omoos ayideemi</t>
+  </si>
+  <si>
+    <t>vae te yarbullhtuk omoos ayideemi</t>
+  </si>
+  <si>
+    <t>vae yaarbullhtuk omoos ayideemi</t>
+  </si>
+  <si>
+    <t>vae gucxattinga omoos ayideemi</t>
+  </si>
+  <si>
+    <t>vae shaama omoos ayideemi</t>
+  </si>
+  <si>
+    <t>jimall ita gali</t>
+  </si>
+  <si>
+    <t>jimall yaara gali</t>
+  </si>
+  <si>
+    <t>jimall yatta gali</t>
+  </si>
+  <si>
+    <t>yaarbullhtuk khita gali</t>
+  </si>
+  <si>
+    <t>yaarbullhtuk ita gali</t>
+  </si>
+  <si>
+    <t>hepullhtuk yaara ccheraan</t>
+  </si>
+  <si>
+    <t>hepullhtuk yatta ccheraan</t>
+  </si>
+  <si>
+    <t>maatto khita ccheraan</t>
+  </si>
+  <si>
+    <t>maatto ita ccheraan</t>
+  </si>
+  <si>
+    <t>maatto yaara ccheremi</t>
+  </si>
+  <si>
+    <t>taene yaara gali</t>
+  </si>
+  <si>
+    <t>taene yatta nemi</t>
+  </si>
+  <si>
+    <t>saattik khita gali</t>
+  </si>
+  <si>
+    <t>saattik ita gali</t>
+  </si>
+  <si>
+    <t>gucxattinga ita nesxh</t>
+  </si>
+  <si>
+    <t>gucxattinga yaara nesxh</t>
+  </si>
+  <si>
+    <t>gucxattinga yatta nesxh</t>
+  </si>
+  <si>
+    <t>doggoiki khita xosxh</t>
+  </si>
+  <si>
+    <t>doggoiki ita xosxh</t>
+  </si>
+  <si>
+    <t>doggoiki yaara xosxh</t>
+  </si>
+  <si>
+    <t>shumshere yaara xosxh</t>
+  </si>
+  <si>
+    <t>shumshere dalla xosxh</t>
+  </si>
+  <si>
+    <t>adite khita gali</t>
+  </si>
+  <si>
+    <t>adite ita gali</t>
+  </si>
+  <si>
+    <t>te yaarbullhtuk yaara gallu</t>
+  </si>
+  <si>
+    <t>te yaarbullhtuk yatta gallu</t>
+  </si>
+  <si>
+    <t>hepullhtuk khita cchurumu</t>
+  </si>
+  <si>
+    <t>hepullhtuk ita cchurumu</t>
+  </si>
+  <si>
+    <t>chamarutto yaara cchurumu</t>
+  </si>
+  <si>
+    <t>chamarutto yatta cchurumu</t>
+  </si>
+  <si>
+    <t>thamene khita gallu</t>
+  </si>
+  <si>
+    <t>thamene ita gallu</t>
+  </si>
+  <si>
+    <t>hepullhtuk yatta walimi</t>
+  </si>
+  <si>
+    <t>hepullhtuk yatta walchimi</t>
+  </si>
+  <si>
+    <t>hepullhtuk yatta wallumbi</t>
+  </si>
+  <si>
+    <t>maatto khita domoomu</t>
+  </si>
+  <si>
+    <t>maatto khita deemi</t>
+  </si>
+  <si>
+    <t>maatto khita deembai</t>
+  </si>
+  <si>
+    <t>maatto khita deembi</t>
+  </si>
+  <si>
+    <t>chakaatto khita domoomu</t>
+  </si>
+  <si>
+    <t>chakaatto khita deemi</t>
+  </si>
+  <si>
+    <t>chakaatto khita deembai</t>
+  </si>
+  <si>
+    <t>chakaatto khita deembi</t>
+  </si>
+  <si>
+    <t>chakaatto yatta walchimi</t>
+  </si>
+  <si>
+    <t>chakaatto yatta wallumbi</t>
+  </si>
+  <si>
+    <t>chamarutto khita domoombu</t>
+  </si>
+  <si>
+    <t>chamarutto khita deemi</t>
+  </si>
+  <si>
+    <t>thamene khita nemu</t>
+  </si>
+  <si>
+    <t>thamene khita neaasccumu</t>
+  </si>
+  <si>
+    <t>thamene khita nembiasccimi</t>
+  </si>
+  <si>
+    <t>shaama yatta walchimi</t>
+  </si>
+  <si>
+    <t>shaama yatta wallumbi</t>
+  </si>
+  <si>
+    <t>bullhtuki khita walchimi</t>
+  </si>
+  <si>
+    <t>bullhtuki khita wallumbi</t>
+  </si>
+  <si>
+    <t>bullhtuki ita domoomu</t>
+  </si>
+  <si>
+    <t>bullhtuki ita deemi</t>
+  </si>
+  <si>
+    <t>gucxattinga khita domoomu</t>
+  </si>
+  <si>
+    <t>gucxattinga khita deemi</t>
+  </si>
+  <si>
+    <t>bullhtuki yatta walchimi</t>
+  </si>
+  <si>
+    <t>bullhtuki yatta wallumbi</t>
+  </si>
+  <si>
+    <t>thape khita domoomu</t>
+  </si>
+  <si>
+    <t>thape khita deemi</t>
+  </si>
+  <si>
+    <t>ccandurare yatta walchimi</t>
+  </si>
+  <si>
+    <t>ccandurare yatta wallumbi</t>
+  </si>
+  <si>
+    <t>angaro khita domoomu</t>
+  </si>
+  <si>
+    <t>angaro khita deemi</t>
+  </si>
+  <si>
+    <t>gogga shakar mayimi</t>
+  </si>
+  <si>
+    <t>momogga bo mayimi</t>
+  </si>
+  <si>
+    <t>momogga ne mayimi</t>
+  </si>
+  <si>
+    <t>Ja durdana cchel phat nete mel bota meyamba</t>
+  </si>
+  <si>
+    <t>Acxhan mani ka yasena ccheran</t>
+  </si>
+  <si>
+    <t>xakune baspur shei</t>
   </si>
   <si>
     <t>Ja acxhan mani ka akhunng pindi ga ccheram</t>
   </si>
   <si>
-    <t>Xakun e ishpit shechumbi</t>
-  </si>
-  <si>
-    <t>Acxhan mani ka sayil a diyashchan</t>
-  </si>
-  <si>
-    <t>Guke hawazing bicca filhal khasxh</t>
-  </si>
-  <si>
-    <t>Baqi maya ka gaaning thum bo tai han shaaski hawazan mishaski ule dua ka te ka kaat kaat alag net etas dua</t>
-  </si>
-  <si>
-    <t>Xo ja ka un hola  ccheran</t>
-  </si>
-  <si>
-    <t>Ja acxho ajo akhosh</t>
-  </si>
-  <si>
-    <t>Ja se xhakun ajo cxham manumbi</t>
+    <t>Xakune ishpit shechumbi</t>
+  </si>
+  <si>
+    <t>Acxhan mani ka sayila diyashchan</t>
+  </si>
+  <si>
+    <t>Guke hawaazing bicca filhal khaasxh</t>
+  </si>
+  <si>
+    <t>Baqi maya ka gaaning thum bo tai han shaaski hawaazan mishaaski ule dua ka te ka kaat kaat alag net etas dua</t>
+  </si>
+  <si>
+    <t>Xo ja ka un hola ccheran</t>
+  </si>
+  <si>
+    <t>Ja acxo ajo akhosh</t>
+  </si>
+  <si>
+    <t>Ja se xakun ajo cxham manumbi</t>
   </si>
   <si>
     <t>Xapaxap guccharchumbai</t>
@@ -218,10 +401,10 @@
     <t>lala bo hal dua shua ba</t>
   </si>
   <si>
-    <t>ja chacha nicchu paqo esarcham ma pareshan amamning shua</t>
-  </si>
-  <si>
-    <t>nega bo senas dua gogga lloll dua</t>
+    <t>ja chacha nicchu paqo esarcham ma pareshan amamaning</t>
+  </si>
+  <si>
+    <t>nega bo senas dua gogga lloll duaa</t>
   </si>
   <si>
     <t>Lay besa akhi guwayumba</t>
@@ -230,25 +413,25 @@
     <t>Khai berozgaar hiren ja</t>
   </si>
   <si>
-    <t>Awa gutey uley shua dua</t>
-  </si>
-  <si>
-    <t>News reporter wagera guwaya rai dua ka... Gute shoa option dua  agar social guawaya rai dua ka</t>
+    <t>Awa gutey ulle shua dua</t>
+  </si>
+  <si>
+    <t>News reporter wagera guwaya rai dua ka, Gute shoa option dua agar social guawaya rai dua ka</t>
   </si>
   <si>
     <t>Akhilchu boka dia ka lip et </t>
   </si>
   <si>
-    <t>Library ule parhai  echumbai</t>
+    <t>Library ulle parhai echumbai</t>
   </si>
   <si>
     <t>Guke saf han ya bicca akhollum yara zehn ule os</t>
   </si>
   <si>
-    <t>Ajo zalim dua jan gute dunia ... Meskatar meti da</t>
-  </si>
-  <si>
-    <t>Awa ja msg etamam internship xarurt dua nukha</t>
+    <t>Ajo zalim dua jan gute dunia ... Mes kattar meti da</t>
+  </si>
+  <si>
+    <t>Awa ja message etamam internship xarurat dua nukkha</t>
   </si>
   <si>
     <t>Khene dost karachi ya bai </t>
@@ -260,28 +443,22 @@
     <t>showa sahi dova</t>
   </si>
   <si>
-    <t>hen dost Germany ga nembai Ms a gandi</t>
-  </si>
-  <si>
-    <t>Le fukkushum guheyamba ley </t>
-  </si>
-  <si>
-    <t>Gogga be negga msj echam</t>
-  </si>
-  <si>
-    <t>Khene bai Karachi um amutk ane bai bokhabar</t>
-  </si>
-  <si>
-    <t>Chachu tasveeran docca guya</t>
-  </si>
-  <si>
-    <t>thek dua ja baring echam</t>
-  </si>
-  <si>
-    <t>Hir showa hir ba lekin basha basha tehan guwayumba baqi showa dova</t>
-  </si>
-  <si>
-    <t>khali gushangia ucchechi guccharchumccek</t>
+    <t>hen dost Germany ga nembai Ms e gandi</t>
+  </si>
+  <si>
+    <t>Gogga be negga message echam</t>
+  </si>
+  <si>
+    <t>Khene bai tollum amutuk ane bai bokhabar</t>
+  </si>
+  <si>
+    <t>Chachaa tasveeran docca guya</t>
+  </si>
+  <si>
+    <t>theek dua ja baring echam</t>
+  </si>
+  <si>
+    <t>Hir showa hir ba lekin basha basha gomoos guwayumba baqi showa ba</t>
   </si>
   <si>
     <t>botan gosulle yanumba ggaan ka</t>
@@ -293,10 +470,7 @@
     <t>fanng nett masqara achumba un</t>
   </si>
   <si>
-    <t>ne hek ajo addellumam ka kollo go tte letter niya ccheraga</t>
-  </si>
-  <si>
-    <t>ne PTI ne sir a bo yek an duam ka</t>
+    <t>ne hek ajo gudellumam ka kollo un</t>
   </si>
   <si>
     <t>fanng daa botta le yah eta</t>
@@ -308,25 +482,16 @@
     <t>dunya khakkarumam le un</t>
   </si>
   <si>
-    <t>chachi ajo gosmallumbu jagga lloll mani</t>
-  </si>
-  <si>
     <t>ja un gosqayamba na le</t>
   </si>
   <si>
-    <t>ja alchine gari chachu</t>
-  </si>
-  <si>
-    <t>goski dua go mo gokhkosh mo bo muyekan duam</t>
-  </si>
-  <si>
-    <t>Le sakht preshaani duva yar</t>
-  </si>
-  <si>
-    <t>Ja field a systtem maimi ka qaburum ka barabar acham </t>
-  </si>
-  <si>
-    <t>Fis fas jagganng mo khush ayechumbu</t>
+    <t>jaa alchine gari ba un</t>
+  </si>
+  <si>
+    <t>Le ajo preshaani duva yaar</t>
+  </si>
+  <si>
+    <t>Fis fas jagganng ne khosh ayechumbai</t>
   </si>
   <si>
     <t>Warcca jaggachi reference api</t>
@@ -335,25 +500,19 @@
     <t>jeet guana senen bumbarak manisxh</t>
   </si>
   <si>
-    <t>bo ttournamentt an duam le</t>
+    <t>bo tournament an duam le</t>
   </si>
   <si>
     <t>Akhi shua shua dia ka docc besa</t>
   </si>
   <si>
-    <t>ajo aski cchurumba shua un</t>
-  </si>
-  <si>
-    <t>Bo ttunn guwanumba le</t>
-  </si>
-  <si>
-    <t>fesxh un echum ba ja bota fusasccam</t>
-  </si>
-  <si>
-    <t>Awa le jeet eta</t>
-  </si>
-  <si>
-    <t>Taus a tteam niyaa</t>
+    <t>ayi cchurumba shua un</t>
+  </si>
+  <si>
+    <t>Bo tunn guwanumba le</t>
+  </si>
+  <si>
+    <t>Tausa ccheraan ne niyaa</t>
   </si>
   <si>
     <t>baring eta be guya nana mukaatt?</t>
@@ -362,61 +521,43 @@
     <t>Jaa men le</t>
   </si>
   <si>
-    <t>daya acho ka botan nuvell</t>
-  </si>
-  <si>
-    <t>go bhabi mogga intternship barabar aye mayundova gote Field a men yar dost ka apaan</t>
-  </si>
-  <si>
-    <t>Ttatta khoosh dunya asxhindova bo khakharchamba</t>
-  </si>
-  <si>
-    <t>Ja anum domoya en</t>
-  </si>
-  <si>
-    <t>thum mene bu in?</t>
-  </si>
-  <si>
-    <t>Gutte  menay dua le jaa recovery email dua gutte</t>
-  </si>
-  <si>
-    <t>saan saan senumam baring echam mukaatt nukkha</t>
+    <t>daaya acho ka botan nuvell</t>
+  </si>
+  <si>
+    <t>Jaa anum diya os</t>
+  </si>
+  <si>
+    <t>thum mene bai in?</t>
+  </si>
+  <si>
+    <t>saan saan senumam baring echam nekaatt nukkha</t>
   </si>
   <si>
     <t>Bo baring echam</t>
   </si>
   <si>
-    <t>ho ayi manundua hek ka baring naekaatt?</t>
-  </si>
-  <si>
-    <t>Basha basha mayun dua</t>
-  </si>
-  <si>
-    <t>khabar yana naeccum</t>
-  </si>
-  <si>
-    <t>un akkhatena ja khosh echamba nukkha</t>
-  </si>
-  <si>
-    <t>un guya baring etas bam besa</t>
-  </si>
-  <si>
-    <t>le yar ja gogga saan senamba le gutte jawab</t>
-  </si>
-  <si>
-    <t>heke eta kkhabar niya gukhar kkhalas et</t>
-  </si>
-  <si>
-    <t>Filhaal kaaman busy ba office olle</t>
-  </si>
-  <si>
-    <t>adit khasxh echam shua </t>
-  </si>
-  <si>
-    <t>ccandurare thappe research paper submit etas dua ajo halaating tight bicca</t>
-  </si>
-  <si>
-    <t>mi maa jua apaan le </t>
+    <t>ho ayi manunduaa hek ka baring nae kaatt?</t>
+  </si>
+  <si>
+    <t>Basha basha mayundua</t>
+  </si>
+  <si>
+    <t>kkhabar yanaa naeccum</t>
+  </si>
+  <si>
+    <t>un akkhatena ja thosxh echamba nukkha</t>
+  </si>
+  <si>
+    <t>un guya baring etaas bam besaa</t>
+  </si>
+  <si>
+    <t>Filhaal kaman busy ba office olle</t>
+  </si>
+  <si>
+    <t>adit khasxh echam shuaa</t>
+  </si>
+  <si>
+    <t>mi maa jua bo llayen</t>
   </si>
   <si>
     <t>guya photo an ya docca akher</t>
@@ -425,64 +566,64 @@
     <t>bo mayimi</t>
   </si>
   <si>
-    <t>ja ka ba akhi pindi yakalla</t>
-  </si>
-  <si>
-    <t>ne berespate dang dimi</t>
-  </si>
-  <si>
-    <t>go buddu dang dimi</t>
-  </si>
-  <si>
-    <t>momo buddu dang dimi</t>
-  </si>
-  <si>
-    <t>ne buddu dang dimi</t>
-  </si>
-  <si>
-    <t>go ccandurare dang dimi</t>
-  </si>
-  <si>
-    <t>momo ccandurare dang dimi</t>
-  </si>
-  <si>
-    <t>ne ccandurare dang dimi</t>
-  </si>
-  <si>
-    <t>go angaro dang dimi</t>
-  </si>
-  <si>
-    <t>momo angaro dang dimi</t>
-  </si>
-  <si>
-    <t>ne angaro dang dimi</t>
-  </si>
-  <si>
-    <t>ve angaro dang dimi</t>
-  </si>
-  <si>
-    <t>ve ccandurare dang dimi</t>
-  </si>
-  <si>
-    <t>ve ajo paisa dia</t>
-  </si>
-  <si>
-    <t>ve angaro omoos dia</t>
-  </si>
-  <si>
-    <t>ve ccandurare omoos dia</t>
-  </si>
-  <si>
-    <t>ve buddu omoos dia</t>
-  </si>
-  <si>
-    <t>ve berespate omoos dia</t>
-  </si>
-  <si>
-    <t>ve addite omoos dia</t>
-  </si>
-  <si>
-    <t>ne shukuru dang dia</t>
+    <t>ja ka baa akhi pindi yakalla</t>
+  </si>
+  <si>
+    <t>nae berespate dang deemi</t>
+  </si>
+  <si>
+    <t>go buddu dang deemi</t>
+  </si>
+  <si>
+    <t>momo buddu dang deemi</t>
+  </si>
+  <si>
+    <t>nae buddu dang deemi</t>
+  </si>
+  <si>
+    <t>go ccandurare dang deemi</t>
+  </si>
+  <si>
+    <t>momo ccandurare dang deemi</t>
+  </si>
+  <si>
+    <t>ne ccandurare dang deemi</t>
+  </si>
+  <si>
+    <t>go angaro dang deemi</t>
+  </si>
+  <si>
+    <t>momo angaro dang deemi</t>
+  </si>
+  <si>
+    <t>nae angaro dang deemi</t>
+  </si>
+  <si>
+    <t>vae angaro dang deemi</t>
+  </si>
+  <si>
+    <t>vae ccandurare dang deemi</t>
+  </si>
+  <si>
+    <t>vae ajo paisa dia</t>
+  </si>
+  <si>
+    <t>vae angaro omoos dia</t>
+  </si>
+  <si>
+    <t>vae ccandurare omoos dia</t>
+  </si>
+  <si>
+    <t>vae buddu omoos dia</t>
+  </si>
+  <si>
+    <t>vae berespate omoos dia</t>
+  </si>
+  <si>
+    <t>vae addite omoos dia</t>
+  </si>
+  <si>
+    <t>nae shukuru dang dia</t>
   </si>
   <si>
     <t>go shumshere dang dia</t>
@@ -491,7 +632,7 @@
     <t>momo shumshere dang dia</t>
   </si>
   <si>
-    <t>ne shumshere dang dia</t>
+    <t>nae shumshere dang dia</t>
   </si>
   <si>
     <t>go addite dang dia</t>
@@ -500,55 +641,58 @@
     <t>momo addite dang dia</t>
   </si>
   <si>
-    <t>ne addite dang dia</t>
+    <t>nae addite dang dia</t>
   </si>
   <si>
     <t>go berespate dang dia</t>
   </si>
   <si>
-    <t>ne negga gadero seni</t>
-  </si>
-  <si>
-    <t>ne momogga gadero seni</t>
-  </si>
-  <si>
-    <t>ne jagga gadero seni</t>
-  </si>
-  <si>
-    <t>ne segga gadero seni</t>
-  </si>
-  <si>
-    <t>ne gogga  seni</t>
-  </si>
-  <si>
-    <t>ne vaegga  seni</t>
-  </si>
-  <si>
-    <t>ne negga  seni</t>
-  </si>
-  <si>
-    <t>ne momogga  seni</t>
-  </si>
-  <si>
-    <t>ne jagga  seni</t>
-  </si>
-  <si>
-    <t>ne segga  seni</t>
-  </si>
-  <si>
-    <t>cchor cchor, han tthuko an biastemi. Se tthuko bahlt yatte nuhurutt bahlt sxhe sxhe biasccimi.</t>
-  </si>
-  <si>
-    <t>Tauruma yahlltary ballhas waw domomu. Mo hun guaacxa tuni niya domombuasccumu. Te yatte botan numuma</t>
-  </si>
-  <si>
-    <t>momo muhlchi tthuko yatta walimi. Ho dunesh etumbu ka guse tthuko behltum neh sxhicxam? Te yatte</t>
-  </si>
-  <si>
-    <t>yary domo tthuko ga qow etumbu ka,  lay tthuko! ajo cxham amanamba han bahllt an khatta lip ataa? te</t>
-  </si>
-  <si>
-    <t>yatte tthuko han lip echa os cchella wali thuman lip ata senumu. </t>
+    <t>nae naegga gadaero seni</t>
+  </si>
+  <si>
+    <t>nae momogga gadaero seni</t>
+  </si>
+  <si>
+    <t>nae jagga gadaero seni</t>
+  </si>
+  <si>
+    <t>nae segga gadaero seni</t>
+  </si>
+  <si>
+    <t>nae gogga seni</t>
+  </si>
+  <si>
+    <t>nae vaegga seni</t>
+  </si>
+  <si>
+    <t>nae naegga seni</t>
+  </si>
+  <si>
+    <t>nae momogga seni</t>
+  </si>
+  <si>
+    <t>nae jagga seni</t>
+  </si>
+  <si>
+    <t>nae saegga seni</t>
+  </si>
+  <si>
+    <t>cchor cchor, han tthuko an biaasccimi. Se tthuko bahlt yatte nuhurutt bahlt sxhe sxhe biasccimi.</t>
+  </si>
+  <si>
+    <t>Tauruma yahlltary ballhas wawen domombu.</t>
+  </si>
+  <si>
+    <t>Mo hun guaacxa tuni niya domombuasccumu. Te yatte botan numuma momo muhlchi tthuko yatta walimi.</t>
+  </si>
+  <si>
+    <t>Ho dunesh etumbu ka guse tthuko behltum net sxhicxam? </t>
+  </si>
+  <si>
+    <t>Te yatte yary domo tthuko ga qow etumbu ka,  lay tthukoo! ajo cxham amanamba han bahllt an khatta lip etaa</t>
+  </si>
+  <si>
+    <t>teytte tthuko han lip echa os cchella wali thuman lip ata senumu. </t>
   </si>
   <si>
     <t>Te yatte tthuko han ka bahllt an khatta lip atimi naa.</t>
@@ -560,52 +704,49 @@
     <t>Han ka lip echa os isxhqa haranga wali nukkha bahna atumu.</t>
   </si>
   <si>
-    <t>Te yatte ballhas wawe tthukoga senumu ka lay tthuko guhlltainge horgo,</t>
-  </si>
-  <si>
-    <t>guyates a chhangi neh lip et ka ajo giyaxcumbiye nukkha yaara tuni wal atumbu.</t>
-  </si>
-  <si>
-    <t>Ho tthuko nachaar ttir nima tang a horgo, yates a chhangi neh te zall achum ka ya phaphara niwall dee tunicha wallumbi.</t>
+    <t>Teytte ballhas wawe tthukoga senumu ka lay tthuko guhlltaing horgo, guyates a chhangi neh lip et ka ajo giyaxcumbiye nukkha yaara tuni wal atumbu.</t>
+  </si>
+  <si>
+    <t>Ho tthuko nachaar ttir nima tainge horgo, yatise chhangi nete zall achum ka ya phaphara niwall dee tunicha wallumbi.</t>
   </si>
   <si>
     <t>Ho wawe ghasxhap yatta pettek nupisha gatt net, ballda net niya traw.</t>
   </si>
   <si>
-    <t>Halle nomo momes wal nomot senumbu ka, un gusay tthuko gha wal guan ja amemo nosar cchuram. </t>
-  </si>
-  <si>
-    <t>Momese shua senumbu. Ballhas waw holla chiraaga, mo momes a botan numuma pettek dishuya tthuko holla dusumbi.</t>
-  </si>
-  <si>
-    <t>Holla duus mo kyaki mogha akhuly tunichi ajo maaza nukkha masqara nomot momo gattunz ekhara nuwell</t>
-  </si>
-  <si>
-    <t>waw mo momes tunicha numuwash gatt atumbi. Tauruma waw holum domombu, domo se tthuko bia nukkha kkhabr yanumu.</t>
-  </si>
-  <si>
-    <t>Tthuko waw masqara nomot momes mo muchar ulle, awa waw! Bi senumbi. Ho waw cxhew, akhuyng boota shua chap gare paqo mani nukkha.</t>
-  </si>
-  <si>
-    <t>Ho waw a dallum jirmani khatta niya dell nithi shua taap netey tthuko bi nukkha momes dumuch te della muwashimbu. </t>
-  </si>
-  <si>
-    <t>Momes cxicxigha muallumbu, boota siya mo waw mogha siya amo manumbu, ja goo gomes ba nukkha, boota siya te dell a kittori motundulum.</t>
-  </si>
-  <si>
-    <t>Ballhas wawe shua domoster chape shua noyu thoro mo not ho qauv atumbu. Do ames ya xo ka akhuyng ajo dokosuljaas ba nukkha. </t>
+    <t>Haalle nomo momes wal nomot senumbu ka, un gusay tthuko gha wal guan ja amemo nosar cchuram. </t>
+  </si>
+  <si>
+    <t>Momese shua senumbu. Ballhas waw holla cheraagga, mo momes a botan numuma pettek dishuya tthuko holla duusumbi.</t>
+  </si>
+  <si>
+    <t>Holla duus mo kyaki mogha akhuly tunichi ajo shua dua nukkha masqara nomot momo gattunz ekhara nuwell waw mo momes tunicha numuwash gatt atumbi.</t>
+  </si>
+  <si>
+    <t>Tauruma waw hollum domombu, domo se tthuko bia nukkha kkhabr yanumbu.</t>
+  </si>
+  <si>
+    <t>Tthuko waw masqara nomot momes mo muchar ulle, awa waaw! Bi senumbi. waw cxhew, akhuyng boota shua chap gare paqo mani nukkha.</t>
+  </si>
+  <si>
+    <t>Ho wawe dallum jirmani khatta niya dell nithi shua taap netey tthuko bi nukkha momes dumuch te della muwashimbu. </t>
+  </si>
+  <si>
+    <t>Momes cxicxigha muallumbu, boota siya mo waw mogha siya amo manumbu, ja goo gomes ba nukkha, boota siya te dell a kittori motundullum.</t>
+  </si>
+  <si>
+    <t>Ballhas wawe shua domoster chape shua noyu thoro mo not ho qauv atumbu. Do ames ya xo ka akhuyng ajo dokoosuljaas ba nukkha. </t>
   </si>
   <si>
     <t>Tthuko ekharinga nuqas deembi. Paqo shua nisxhi, chhap a thoromo shua nusxhu waw mogha senumbi ka, waw! Ja haryasxh diya.</t>
   </si>
   <si>
-    <t>Waw senumuka, ya neh shohllty noko gatt yatte nuharya xo da bo simba paqo gosera. Tthuko cxhew nima ekharinga shua nuqas hainn atumbi.</t>
-  </si>
-  <si>
-    <t>Shohlty nee sam cce dee waw mogga qaw etumbi, do waw! Go gomes mo gattunz ja nuwel gomes tunicha muwashiyamam. </t>
-  </si>
-  <si>
-    <t>Go lloll ya amota, jaa shua musxhiya, achuma akhilchu akhollum elja senumbi.</t>
+    <t>Wawe senumu ka ya neh shohllty noko gatt yatte nuharya xo da bo simba paqo gosera. Tthuko cxhew nima ekharinga shua nuqas hainn atumbi.</t>
+  </si>
+  <si>
+    <t>Shohllty nee sam cce dee waw mogga qaw etumbi, do waw! Go gomes mo gattunz ja nuwell gomes tunicha muwashiyamam. </t>
+  </si>
+  <si>
+    <t>Go lloll ya amota, jaa shua musxhiya, echuma akhilchu doroing akhollum elja senumbi.</t>
   </si>
   <si>
     <t>Ho waw halle cxicxigha muwallumbu, amutu un mena fat gochamba, un masqara nat ja ames musxhimba nukkha. </t>
@@ -623,13 +764,13 @@
     <t>momogga paqo amuwa</t>
   </si>
   <si>
-    <t>negga paqo uwa</t>
-  </si>
-  <si>
-    <t>negga paqo ayuwa</t>
-  </si>
-  <si>
-    <t>momogga hoi ita</t>
+    <t>naegga paqo uwa</t>
+  </si>
+  <si>
+    <t>naegga paqo ayuwa</t>
+  </si>
+  <si>
+    <t>momogga hoi eta</t>
   </si>
   <si>
     <t>momogga hoi cchuwa</t>
@@ -638,13 +779,13 @@
     <t>momogga hoi dicca</t>
   </si>
   <si>
-    <t>negga hoi ita</t>
-  </si>
-  <si>
-    <t>negga hoi cchuwa</t>
-  </si>
-  <si>
-    <t>negga hoi dicca</t>
+    <t>naegga hoi eta</t>
+  </si>
+  <si>
+    <t>naegga hoi cchuwa</t>
+  </si>
+  <si>
+    <t>naegga hoi dicca</t>
   </si>
   <si>
     <t>momogga girinj ita</t>
@@ -656,7 +797,7 @@
     <t>momogga girinj dicca</t>
   </si>
   <si>
-    <t>negga girinj ita</t>
+    <t>naegga girinj ita</t>
   </si>
   <si>
     <t>momogga wallhte mayimi</t>
@@ -1058,34 +1199,19 @@
     <t>bo zali ba ?  akhuing ajo shua gunz an dua gute shahar ka ajo shua shahar an dua</t>
   </si>
   <si>
-    <t>ayash gulabi isxhqam manumbi akhuing</t>
-  </si>
-  <si>
     <t>paqo sxhe cardboard ayi sxhe</t>
   </si>
   <si>
-    <t>Le halles sena go bo doro dua</t>
-  </si>
-  <si>
     <t>ja ka un neme te ddoro net cchuren</t>
   </si>
   <si>
     <t>ja acce bo bika gogga gucham</t>
   </si>
   <si>
-    <t>ja sattik khela neyamam ajo maza diya jagga ne nnyu halles ajo wali</t>
-  </si>
-  <si>
-    <t>ja gogga han baran siyama agar ggafa akuwayumba ka</t>
-  </si>
-  <si>
     <t>un ajo gukhar thathall ayet be ka</t>
   </si>
   <si>
     <t>Javayu 100 ggaring har jawane itas dua le akhuyng sham khasxh</t>
-  </si>
-  <si>
-    <t>Bess aye sxhe chhap she</t>
   </si>
   <si>
     <t>ne sheghitan mull cce dis na darkut bull cce dis</t>
@@ -1151,9 +1277,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -1191,7 +1317,83 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1206,31 +1408,16 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1244,76 +1431,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1322,6 +1441,13 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1336,37 +1462,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1378,31 +1474,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1420,19 +1522,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1444,7 +1558,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1456,7 +1606,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1468,55 +1636,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1527,6 +1653,65 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1547,68 +1732,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1630,7 +1756,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1648,136 +1774,139 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2042,159 +2171,159 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:A1000"/>
+  <dimension ref="A1:A1042"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A237" workbookViewId="0">
+      <selection activeCell="A260" sqref="A260"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4259259259259" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="103.138888888889" customWidth="1"/>
+    <col min="1" max="1" width="164.111111111111" customWidth="1"/>
     <col min="2" max="6" width="14.4259259259259" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1" spans="1:1">
+    <row r="1" customHeight="1" spans="1:1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1" spans="1:1">
+    <row r="2" customHeight="1" spans="1:1">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" ht="15.75" customHeight="1" spans="1:1">
+    <row r="3" customHeight="1" spans="1:1">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" ht="15.75" customHeight="1" spans="1:1">
+    <row r="4" customHeight="1" spans="1:1">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" ht="15.75" customHeight="1" spans="1:1">
+    <row r="5" customHeight="1" spans="1:1">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" ht="15.75" customHeight="1" spans="1:1">
+    <row r="6" customHeight="1" spans="1:1">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" ht="15.75" customHeight="1" spans="1:1">
+    <row r="7" customHeight="1" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" ht="15.75" customHeight="1" spans="1:1">
+    <row r="8" customHeight="1" spans="1:1">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" ht="15.75" customHeight="1" spans="1:1">
+    <row r="9" customHeight="1" spans="1:1">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" ht="15.75" customHeight="1" spans="1:1">
+    <row r="10" customHeight="1" spans="1:1">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" ht="15.75" customHeight="1" spans="1:1">
+    <row r="11" customHeight="1" spans="1:1">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" ht="15.75" customHeight="1" spans="1:1">
+    <row r="12" customHeight="1" spans="1:1">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" ht="15.75" customHeight="1" spans="1:1">
+    <row r="13" customHeight="1" spans="1:1">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" ht="15.75" customHeight="1" spans="1:1">
+    <row r="14" customHeight="1" spans="1:1">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" ht="15.75" customHeight="1" spans="1:1">
+    <row r="15" customHeight="1" spans="1:1">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" ht="15.75" customHeight="1" spans="1:1">
+    <row r="16" customHeight="1" spans="1:1">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" ht="15.75" customHeight="1" spans="1:1">
+    <row r="17" customHeight="1" spans="1:1">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" ht="15.75" customHeight="1" spans="1:1">
+    <row r="18" customHeight="1" spans="1:1">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" ht="15.75" customHeight="1" spans="1:1">
+    <row r="19" customHeight="1" spans="1:1">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" ht="15.75" customHeight="1" spans="1:1">
+    <row r="20" customHeight="1" spans="1:1">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" ht="15.75" customHeight="1" spans="1:1">
+    <row r="21" customHeight="1" spans="1:1">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" ht="15.75" customHeight="1" spans="1:1">
+    <row r="22" customHeight="1" spans="1:1">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" ht="15.75" customHeight="1" spans="1:1">
+    <row r="23" customHeight="1" spans="1:1">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" ht="15.75" customHeight="1" spans="1:1">
+    <row r="24" customHeight="1" spans="1:1">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" ht="15.75" customHeight="1" spans="1:1">
+    <row r="25" customHeight="1" spans="1:1">
       <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" ht="15.75" customHeight="1" spans="1:1">
+    <row r="26" customHeight="1" spans="1:1">
       <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" ht="15.75" customHeight="1" spans="1:1">
+    <row r="27" customHeight="1" spans="1:1">
       <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" ht="15.75" customHeight="1" spans="1:1">
+    <row r="28" customHeight="1" spans="1:1">
       <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" ht="15.75" customHeight="1" spans="1:1">
+    <row r="29" customHeight="1" spans="1:1">
       <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
@@ -2615,1345 +2744,1525 @@
       </c>
     </row>
     <row r="113" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A113" s="2" t="s">
+      <c r="A113" s="3" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="114" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A114" s="2" t="s">
+      <c r="A114" s="3" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="115" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A115" s="2" t="s">
+      <c r="A115" s="3" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="116" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A116" s="2" t="s">
+      <c r="A116" s="3" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="117" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A117" s="2" t="s">
+      <c r="A117" s="3" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="118" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A118" s="2" t="s">
+      <c r="A118" s="3" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="119" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A119" s="2" t="s">
+      <c r="A119" s="3" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="120" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A120" s="2" t="s">
+      <c r="A120" s="3" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="121" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A121" s="2" t="s">
+      <c r="A121" s="3" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="122" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A122" s="2" t="s">
+      <c r="A122" s="3" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="123" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A123" s="2" t="s">
+      <c r="A123" s="3" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="124" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A124" s="2" t="s">
+      <c r="A124" s="3" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="125" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A125" s="2" t="s">
+      <c r="A125" s="3" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="126" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A126" s="2" t="s">
+      <c r="A126" s="3" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="127" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A127" s="2" t="s">
+      <c r="A127" s="3" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="128" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A128" s="2" t="s">
+      <c r="A128" s="3" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="129" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A129" s="2" t="s">
+      <c r="A129" s="3" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="130" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A130" s="2" t="s">
+      <c r="A130" s="3" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="131" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A131" s="2" t="s">
+      <c r="A131" s="3" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="132" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A132" s="2" t="s">
+      <c r="A132" s="3" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="133" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A133" s="2" t="s">
-        <v>97</v>
+      <c r="A133" s="3" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="134" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A134" s="2" t="s">
-        <v>132</v>
+      <c r="A134" s="3" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="135" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A135" s="2" t="s">
-        <v>133</v>
+      <c r="A135" s="3" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="136" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A136" s="2" t="s">
-        <v>134</v>
+      <c r="A136" s="3" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="137" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A137" s="2" t="s">
-        <v>135</v>
+      <c r="A137" s="3" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="138" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A138" s="2" t="s">
-        <v>136</v>
+      <c r="A138" s="3" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="139" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A139" s="2" t="s">
-        <v>137</v>
+      <c r="A139" s="3" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="140" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A140" s="2" t="s">
-        <v>138</v>
+      <c r="A140" s="3" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="141" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A141" s="2" t="s">
-        <v>139</v>
+      <c r="A141" s="3" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="142" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A142" s="2" t="s">
-        <v>140</v>
+      <c r="A142" s="3" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="143" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A143" s="2" t="s">
-        <v>141</v>
+      <c r="A143" s="3" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="144" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A144" s="2" t="s">
-        <v>142</v>
+      <c r="A144" s="3" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="145" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A145" s="2" t="s">
-        <v>143</v>
+      <c r="A145" s="3" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="146" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A146" s="2" t="s">
-        <v>144</v>
+      <c r="A146" s="3" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="147" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A147" s="2" t="s">
-        <v>145</v>
+      <c r="A147" s="3" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="148" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A148" s="2" t="s">
-        <v>146</v>
+      <c r="A148" s="3" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="149" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A149" s="2" t="s">
-        <v>147</v>
+      <c r="A149" s="3" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="150" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A150" s="2" t="s">
-        <v>148</v>
+      <c r="A150" s="3" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="151" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A151" s="2" t="s">
-        <v>149</v>
+      <c r="A151" s="3" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="152" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A152" s="2" t="s">
-        <v>150</v>
+      <c r="A152" s="3" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="153" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A153" s="2" t="s">
-        <v>151</v>
+      <c r="A153" s="3" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="154" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A154" s="2" t="s">
-        <v>152</v>
+      <c r="A154" s="3" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="155" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A155" s="2" t="s">
-        <v>153</v>
+      <c r="A155" s="3" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="156" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A156" s="2" t="s">
-        <v>154</v>
+      <c r="A156" s="3" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="157" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A157" s="2" t="s">
-        <v>155</v>
+      <c r="A157" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="158" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A158" s="2" t="s">
-        <v>156</v>
+      <c r="A158" s="3" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="159" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A159" s="2" t="s">
-        <v>157</v>
+      <c r="A159" s="3" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="160" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A160" s="2" t="s">
-        <v>158</v>
+      <c r="A160" s="3" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="161" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A161" s="2" t="s">
-        <v>159</v>
+      <c r="A161" s="3" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="162" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A162" s="2" t="s">
-        <v>160</v>
+      <c r="A162" s="3" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="163" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A163" s="2" t="s">
-        <v>161</v>
+      <c r="A163" s="3" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="164" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A164" s="2" t="s">
-        <v>162</v>
+      <c r="A164" s="3" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="165" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A165" s="2" t="s">
-        <v>163</v>
+      <c r="A165" s="3" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="166" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A166" s="2" t="s">
-        <v>164</v>
+      <c r="A166" s="3" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="167" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A167" s="2" t="s">
-        <v>165</v>
+      <c r="A167" s="3" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="168" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A168" s="2" t="s">
-        <v>166</v>
+      <c r="A168" s="3" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="169" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A169" s="2" t="s">
-        <v>166</v>
+      <c r="A169" s="3" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="170" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A170" s="2" t="s">
-        <v>167</v>
+      <c r="A170" s="3" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="171" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A171" s="2" t="s">
-        <v>168</v>
+      <c r="A171" s="3" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="172" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A172" s="2" t="s">
-        <v>169</v>
+      <c r="A172" s="3" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="173" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A173" s="2" t="s">
-        <v>170</v>
+      <c r="A173" s="3" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="174" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A174" s="2" t="s">
-        <v>171</v>
+      <c r="A174" s="3" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="175" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A175" s="2" t="s">
-        <v>172</v>
+      <c r="A175" s="3" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="176" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A176" s="2" t="s">
-        <v>172</v>
+      <c r="A176" s="3" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="177" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A177" s="2" t="s">
-        <v>173</v>
+      <c r="A177" s="3" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="178" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A178" s="2" t="s">
-        <v>174</v>
+      <c r="A178" s="3" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="179" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A179" s="2" t="s">
-        <v>175</v>
+      <c r="A179" s="3" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="180" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A180" s="2" t="s">
-        <v>176</v>
+      <c r="A180" s="3" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="181" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A181" s="2" t="s">
-        <v>177</v>
+      <c r="A181" s="3" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="182" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A182" s="2" t="s">
-        <v>178</v>
+      <c r="A182" s="3" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="183" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A183" s="2" t="s">
-        <v>179</v>
+      <c r="A183" s="3" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="184" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A184" s="2" t="s">
-        <v>180</v>
+      <c r="A184" s="3" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="185" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A185" s="2" t="s">
-        <v>181</v>
+      <c r="A185" s="3" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="186" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A186" s="2" t="s">
-        <v>182</v>
+      <c r="A186" s="3" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="187" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A187" s="2" t="s">
-        <v>183</v>
+      <c r="A187" s="3" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="188" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A188" s="2" t="s">
-        <v>184</v>
+      <c r="A188" s="3" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="189" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A189" s="2" t="s">
-        <v>185</v>
+      <c r="A189" s="3" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="190" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A190" s="2" t="s">
-        <v>186</v>
+      <c r="A190" s="3" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="191" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A191" s="2" t="s">
-        <v>187</v>
+      <c r="A191" s="3" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="192" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A192" s="2" t="s">
-        <v>188</v>
+      <c r="A192" s="3" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="193" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A193" s="2" t="s">
-        <v>189</v>
+      <c r="A193" s="3" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="194" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A194" s="2" t="s">
-        <v>190</v>
+      <c r="A194" s="3" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="195" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A195" s="2" t="s">
-        <v>191</v>
+      <c r="A195" s="3" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="196" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A196" s="2" t="s">
-        <v>192</v>
+      <c r="A196" s="3" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="197" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A197" s="2" t="s">
-        <v>193</v>
+      <c r="A197" s="3" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="198" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A198" s="2" t="s">
-        <v>194</v>
+      <c r="A198" s="3" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="199" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A199" s="2" t="s">
-        <v>195</v>
+      <c r="A199" s="3" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="200" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A200" s="2" t="s">
-        <v>196</v>
+      <c r="A200" s="3" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="201" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A201" s="2" t="s">
-        <v>197</v>
+      <c r="A201" s="3" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="202" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A202" s="2" t="s">
-        <v>198</v>
+      <c r="A202" s="3" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="203" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A203" s="2" t="s">
-        <v>199</v>
+      <c r="A203" s="3" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="204" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A204" s="2" t="s">
-        <v>200</v>
+      <c r="A204" s="3" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="205" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A205" s="2" t="s">
-        <v>201</v>
+      <c r="A205" s="3" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="206" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A206" s="2" t="s">
-        <v>202</v>
+      <c r="A206" s="3" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="207" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A207" s="2" t="s">
-        <v>203</v>
+      <c r="A207" s="3" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="208" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A208" s="2" t="s">
-        <v>204</v>
+      <c r="A208" s="3" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="209" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A209" s="2" t="s">
-        <v>205</v>
+      <c r="A209" s="3" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="210" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A210" s="2" t="s">
-        <v>206</v>
+      <c r="A210" s="3" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="211" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A211" s="2" t="s">
-        <v>207</v>
+      <c r="A211" s="3" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="212" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A212" s="2" t="s">
-        <v>208</v>
+      <c r="A212" s="3" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="213" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A213" s="2" t="s">
-        <v>209</v>
+      <c r="A213" s="3" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="214" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A214" s="2" t="s">
-        <v>210</v>
+      <c r="A214" s="3" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="215" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A215" s="2" t="s">
-        <v>211</v>
+      <c r="A215" s="3" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="216" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A216" s="2" t="s">
-        <v>212</v>
+      <c r="A216" s="3" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="217" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A217" s="2" t="s">
-        <v>213</v>
+      <c r="A217" s="3" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="218" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A218" s="2" t="s">
-        <v>214</v>
+      <c r="A218" s="3" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="219" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A219" s="2" t="s">
-        <v>215</v>
+      <c r="A219" s="3" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="220" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A220" s="2" t="s">
-        <v>216</v>
+      <c r="A220" s="3" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="221" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A221" s="2" t="s">
-        <v>217</v>
+      <c r="A221" s="3" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="222" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A222" s="2" t="s">
-        <v>218</v>
+      <c r="A222" s="3" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="223" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A223" s="2" t="s">
-        <v>219</v>
+      <c r="A223" s="3" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="224" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A224" s="2" t="s">
-        <v>220</v>
+      <c r="A224" s="3" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="225" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A225" s="2" t="s">
-        <v>221</v>
+      <c r="A225" s="3" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="226" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A226" s="2" t="s">
-        <v>222</v>
+      <c r="A226" s="3" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="227" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A227" s="2" t="s">
-        <v>223</v>
+      <c r="A227" s="3" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="228" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A228" s="2" t="s">
-        <v>224</v>
+      <c r="A228" s="3" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="229" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A229" s="2" t="s">
-        <v>225</v>
+      <c r="A229" s="3" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="230" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A230" s="2" t="s">
-        <v>226</v>
+      <c r="A230" s="3" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="231" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A231" s="2" t="s">
-        <v>227</v>
+      <c r="A231" s="3" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="232" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A232" s="2" t="s">
-        <v>228</v>
+      <c r="A232" s="3" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="233" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A233" s="2" t="s">
-        <v>229</v>
+      <c r="A233" s="3" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="234" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A234" s="2" t="s">
-        <v>230</v>
+      <c r="A234" s="3" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="235" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A235" s="2" t="s">
-        <v>231</v>
+      <c r="A235" s="3" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="236" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A236" s="2" t="s">
-        <v>232</v>
+      <c r="A236" s="3" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="237" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A237" s="2" t="s">
-        <v>233</v>
+      <c r="A237" s="3" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="238" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A238" s="2" t="s">
-        <v>234</v>
+      <c r="A238" s="3" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="239" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A239" s="2" t="s">
-        <v>235</v>
+      <c r="A239" s="3" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="240" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A240" s="2" t="s">
-        <v>236</v>
+      <c r="A240" s="3" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="241" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A241" s="2" t="s">
-        <v>237</v>
+      <c r="A241" s="3" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="242" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A242" s="2" t="s">
-        <v>238</v>
+      <c r="A242" s="3" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="243" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A243" s="2" t="s">
-        <v>239</v>
+      <c r="A243" s="3" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="244" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A244" s="2" t="s">
-        <v>240</v>
+      <c r="A244" s="3" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="245" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A245" s="2" t="s">
-        <v>241</v>
+      <c r="A245" s="3" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="246" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A246" s="2" t="s">
-        <v>242</v>
+      <c r="A246" s="3" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="247" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A247" s="2" t="s">
-        <v>243</v>
+      <c r="A247" s="3" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="248" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A248" s="2" t="s">
-        <v>244</v>
+      <c r="A248" s="3" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="249" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A249" s="2" t="s">
-        <v>245</v>
+      <c r="A249" s="3" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="250" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A250" s="2" t="s">
-        <v>246</v>
+      <c r="A250" s="3" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="251" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A251" s="2" t="s">
-        <v>247</v>
+      <c r="A251" s="3" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="252" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A252" s="2" t="s">
-        <v>248</v>
+      <c r="A252" s="3" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="253" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A253" s="2" t="s">
-        <v>249</v>
+      <c r="A253" s="3" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="254" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A254" s="2" t="s">
-        <v>250</v>
+      <c r="A254" s="3" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="255" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A255" s="2" t="s">
-        <v>251</v>
+      <c r="A255" s="3" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="256" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A256" s="2" t="s">
-        <v>252</v>
+      <c r="A256" s="3" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="257" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A257" s="2" t="s">
-        <v>253</v>
+      <c r="A257" s="3" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="258" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A258" s="2" t="s">
-        <v>254</v>
+      <c r="A258" s="3" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="259" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A259" s="2" t="s">
-        <v>255</v>
+      <c r="A259" s="3" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="260" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A260" s="2" t="s">
-        <v>256</v>
+      <c r="A260" s="3" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="261" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A261" s="2" t="s">
-        <v>257</v>
+      <c r="A261" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="262" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A262" s="2" t="s">
-        <v>258</v>
+      <c r="A262" s="3" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="263" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A263" s="2" t="s">
-        <v>259</v>
+      <c r="A263" s="3" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="264" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A264" s="2" t="s">
-        <v>260</v>
+      <c r="A264" s="3" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="265" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A265" s="2" t="s">
-        <v>261</v>
+      <c r="A265" s="3" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="266" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A266" s="2" t="s">
-        <v>262</v>
+      <c r="A266" s="3" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="267" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A267" s="2" t="s">
-        <v>263</v>
+      <c r="A267" s="3" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="268" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A268" s="2" t="s">
-        <v>264</v>
+      <c r="A268" s="3" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="269" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A269" s="2" t="s">
-        <v>265</v>
+      <c r="A269" s="3" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="270" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A270" s="2" t="s">
-        <v>266</v>
+      <c r="A270" s="3" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="271" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A271" s="2" t="s">
-        <v>267</v>
+      <c r="A271" s="3" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="272" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A272" s="2" t="s">
-        <v>268</v>
+      <c r="A272" s="3" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="273" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A273" s="2" t="s">
-        <v>269</v>
+      <c r="A273" s="3" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="274" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A274" s="2" t="s">
-        <v>270</v>
+      <c r="A274" s="3" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="275" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A275" s="2" t="s">
-        <v>271</v>
+      <c r="A275" s="3" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="276" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A276" s="2" t="s">
-        <v>272</v>
+      <c r="A276" s="3" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="277" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A277" s="2" t="s">
-        <v>273</v>
+      <c r="A277" s="3" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="278" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A278" s="2" t="s">
-        <v>274</v>
+      <c r="A278" s="3" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="279" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A279" s="2" t="s">
-        <v>275</v>
+      <c r="A279" s="3" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="280" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A280" s="2" t="s">
-        <v>276</v>
+      <c r="A280" s="3" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="281" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A281" s="2" t="s">
-        <v>277</v>
+      <c r="A281" s="3" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="282" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A282" s="2" t="s">
-        <v>278</v>
+      <c r="A282" s="3" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="283" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A283" s="2" t="s">
-        <v>279</v>
+      <c r="A283" s="3" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="284" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A284" s="2" t="s">
-        <v>280</v>
+      <c r="A284" s="3" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="285" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A285" s="2" t="s">
-        <v>281</v>
+      <c r="A285" s="3" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="286" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A286" s="2" t="s">
-        <v>282</v>
+      <c r="A286" s="3" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="287" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A287" s="2" t="s">
-        <v>283</v>
+      <c r="A287" s="3" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="288" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A288" s="2" t="s">
-        <v>284</v>
+      <c r="A288" s="3" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="289" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A289" s="2" t="s">
-        <v>285</v>
+      <c r="A289" s="3" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="290" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A290" s="2" t="s">
-        <v>286</v>
+      <c r="A290" s="3" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="291" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A291" s="2" t="s">
-        <v>287</v>
+      <c r="A291" s="3" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="292" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A292" s="2" t="s">
-        <v>288</v>
+      <c r="A292" s="3" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="293" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A293" s="2" t="s">
-        <v>289</v>
+      <c r="A293" s="3" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="294" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A294" s="2" t="s">
-        <v>290</v>
+      <c r="A294" s="3" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="295" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A295" s="2" t="s">
-        <v>291</v>
+      <c r="A295" s="3" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="296" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A296" s="2" t="s">
-        <v>292</v>
+      <c r="A296" s="3" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="297" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A297" s="2" t="s">
-        <v>293</v>
+      <c r="A297" s="3" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="298" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A298" s="2" t="s">
-        <v>294</v>
+      <c r="A298" s="3" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="299" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A299" s="2" t="s">
-        <v>295</v>
+      <c r="A299" s="3" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="300" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A300" s="2" t="s">
-        <v>296</v>
+      <c r="A300" s="3" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="301" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A301" s="2" t="s">
-        <v>297</v>
+      <c r="A301" s="3" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="302" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A302" s="2" t="s">
-        <v>298</v>
+      <c r="A302" s="3" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="303" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A303" s="2" t="s">
-        <v>299</v>
+      <c r="A303" s="3" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="304" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A304" s="2" t="s">
-        <v>300</v>
+      <c r="A304" s="3" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="305" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A305" s="2" t="s">
-        <v>301</v>
+      <c r="A305" s="3" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="306" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A306" s="2" t="s">
-        <v>302</v>
+      <c r="A306" s="3" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="307" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A307" s="2" t="s">
-        <v>303</v>
+      <c r="A307" s="3" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="308" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A308" s="2" t="s">
-        <v>304</v>
+      <c r="A308" s="3" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="309" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A309" s="2" t="s">
-        <v>305</v>
+      <c r="A309" s="3" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="310" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A310" s="2" t="s">
-        <v>306</v>
+      <c r="A310" s="3" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="311" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A311" s="2" t="s">
-        <v>307</v>
+      <c r="A311" s="3" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="312" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A312" s="2" t="s">
-        <v>308</v>
+      <c r="A312" s="3" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="313" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A313" s="2" t="s">
-        <v>309</v>
+      <c r="A313" s="3" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="314" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A314" s="2" t="s">
-        <v>310</v>
+      <c r="A314" s="3" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="315" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A315" s="2" t="s">
-        <v>311</v>
+      <c r="A315" s="3" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="316" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A316" s="2" t="s">
-        <v>312</v>
+      <c r="A316" s="3" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="317" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A317" s="2" t="s">
-        <v>313</v>
+      <c r="A317" s="3" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="318" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A318" s="2" t="s">
-        <v>314</v>
+      <c r="A318" s="3" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="319" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A319" s="2" t="s">
-        <v>315</v>
+      <c r="A319" s="3" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="320" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A320" s="2" t="s">
-        <v>316</v>
+      <c r="A320" s="3" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="321" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A321" s="2" t="s">
-        <v>317</v>
+      <c r="A321" s="3" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="322" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A322" s="2" t="s">
-        <v>318</v>
+      <c r="A322" s="3" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="323" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A323" s="2" t="s">
-        <v>319</v>
+      <c r="A323" s="3" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="324" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A324" s="2" t="s">
-        <v>320</v>
+      <c r="A324" s="3" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="325" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A325" s="2" t="s">
-        <v>321</v>
+      <c r="A325" s="3" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="326" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A326" s="2" t="s">
-        <v>322</v>
+      <c r="A326" s="3" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="327" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A327" s="2" t="s">
-        <v>323</v>
+      <c r="A327" s="3" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="328" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A328" s="2" t="s">
-        <v>324</v>
+      <c r="A328" s="3" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="329" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A329" s="2" t="s">
-        <v>325</v>
+      <c r="A329" s="3" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="330" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A330" s="2" t="s">
-        <v>326</v>
+      <c r="A330" s="3" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="331" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A331" s="2" t="s">
-        <v>327</v>
+      <c r="A331" s="3" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="332" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A332" s="2" t="s">
-        <v>328</v>
+      <c r="A332" s="3" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="333" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A333" s="2" t="s">
-        <v>329</v>
+      <c r="A333" s="3" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="334" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A334" s="2" t="s">
-        <v>330</v>
+      <c r="A334" s="3" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="335" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A335" s="2" t="s">
-        <v>331</v>
+      <c r="A335" s="3" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="336" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A336" s="2" t="s">
-        <v>332</v>
+      <c r="A336" s="3" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="337" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A337" s="2" t="s">
-        <v>333</v>
+      <c r="A337" s="3" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="338" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A338" s="2" t="s">
-        <v>334</v>
+      <c r="A338" s="3" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="339" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A339" s="2" t="s">
-        <v>335</v>
+      <c r="A339" s="3" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="340" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A340" s="2" t="s">
-        <v>336</v>
+      <c r="A340" s="3" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="341" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A341" s="2" t="s">
-        <v>337</v>
+      <c r="A341" s="3" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="342" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A342" s="2" t="s">
-        <v>338</v>
+      <c r="A342" s="3" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="343" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A343" s="2" t="s">
-        <v>339</v>
+      <c r="A343" s="3" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="344" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A344" s="2" t="s">
-        <v>340</v>
+      <c r="A344" s="3" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="345" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A345" s="2" t="s">
-        <v>341</v>
+      <c r="A345" s="3" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="346" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A346" s="2" t="s">
-        <v>342</v>
+      <c r="A346" s="3" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="347" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A347" s="2" t="s">
-        <v>343</v>
+      <c r="A347" s="3" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="348" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A348" s="2" t="s">
-        <v>344</v>
+      <c r="A348" s="3" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="349" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A349" s="2" t="s">
-        <v>345</v>
+      <c r="A349" s="3" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="350" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A350" s="2" t="s">
-        <v>346</v>
+      <c r="A350" s="3" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="351" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A351" s="2" t="s">
-        <v>347</v>
+      <c r="A351" s="3" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="352" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A352" s="2" t="s">
-        <v>348</v>
+      <c r="A352" s="3" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="353" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A353" s="2" t="s">
-        <v>349</v>
+      <c r="A353" s="3" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="354" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A354" s="2" t="s">
-        <v>350</v>
+      <c r="A354" s="3" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="355" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A355" s="2" t="s">
-        <v>351</v>
+      <c r="A355" s="3" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="356" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A356" s="2" t="s">
-        <v>352</v>
+      <c r="A356" s="3" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="357" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A357" s="2" t="s">
-        <v>353</v>
+      <c r="A357" s="3" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="358" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A358" s="2" t="s">
-        <v>354</v>
+      <c r="A358" s="3" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="359" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A359" s="2" t="s">
-        <v>355</v>
+      <c r="A359" s="3" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="360" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A360" s="2" t="s">
-        <v>356</v>
+      <c r="A360" s="3" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="361" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A361" s="2" t="s">
-        <v>357</v>
+      <c r="A361" s="3" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="362" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A362" s="2" t="s">
-        <v>358</v>
+      <c r="A362" s="3" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="363" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A363" s="2" t="s">
-        <v>359</v>
+      <c r="A363" s="3" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="364" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A364" s="2" t="s">
-        <v>360</v>
+      <c r="A364" s="3" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="365" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A365" s="2" t="s">
-        <v>361</v>
+      <c r="A365" s="3" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="366" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A366" s="2" t="s">
-        <v>362</v>
+      <c r="A366" s="3" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="367" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A367" s="2" t="s">
-        <v>363</v>
+      <c r="A367" s="3" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="368" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A368" s="2" t="s">
-        <v>364</v>
+      <c r="A368" s="3" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="369" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A369" s="2" t="s">
-        <v>365</v>
+      <c r="A369" s="3" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="370" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A370" s="2" t="s">
-        <v>366</v>
+      <c r="A370" s="3" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="371" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A371" s="2" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="372" ht="15.75" customHeight="1"/>
-    <row r="373" ht="15.75" customHeight="1"/>
-    <row r="374" ht="15.75" customHeight="1"/>
-    <row r="375" ht="15.75" customHeight="1"/>
-    <row r="376" ht="15.75" customHeight="1"/>
-    <row r="377" ht="15.75" customHeight="1"/>
-    <row r="378" ht="15.75" customHeight="1"/>
-    <row r="379" ht="15.75" customHeight="1"/>
-    <row r="380" ht="15.75" customHeight="1"/>
-    <row r="381" ht="15.75" customHeight="1"/>
-    <row r="382" ht="15.75" customHeight="1"/>
-    <row r="383" ht="15.75" customHeight="1"/>
-    <row r="384" ht="15.75" customHeight="1"/>
-    <row r="385" ht="15.75" customHeight="1"/>
-    <row r="386" ht="15.75" customHeight="1"/>
-    <row r="387" ht="15.75" customHeight="1"/>
-    <row r="388" ht="15.75" customHeight="1"/>
-    <row r="389" ht="15.75" customHeight="1"/>
-    <row r="390" ht="15.75" customHeight="1"/>
-    <row r="391" ht="15.75" customHeight="1"/>
-    <row r="392" ht="15.75" customHeight="1"/>
-    <row r="393" ht="15.75" customHeight="1"/>
-    <row r="394" ht="15.75" customHeight="1"/>
-    <row r="395" ht="15.75" customHeight="1"/>
-    <row r="396" ht="15.75" customHeight="1"/>
-    <row r="397" ht="15.75" customHeight="1"/>
-    <row r="398" ht="15.75" customHeight="1"/>
-    <row r="399" ht="15.75" customHeight="1"/>
-    <row r="400" ht="15.75" customHeight="1"/>
-    <row r="401" ht="15.75" customHeight="1"/>
-    <row r="402" ht="15.75" customHeight="1"/>
-    <row r="403" ht="15.75" customHeight="1"/>
-    <row r="404" ht="15.75" customHeight="1"/>
-    <row r="405" ht="15.75" customHeight="1"/>
-    <row r="406" ht="15.75" customHeight="1"/>
-    <row r="407" ht="15.75" customHeight="1"/>
-    <row r="408" ht="15.75" customHeight="1"/>
-    <row r="409" ht="15.75" customHeight="1"/>
-    <row r="410" ht="15.75" customHeight="1"/>
-    <row r="411" ht="15.75" customHeight="1"/>
-    <row r="412" ht="15.75" customHeight="1"/>
-    <row r="413" ht="15.75" customHeight="1"/>
-    <row r="414" ht="15.75" customHeight="1"/>
-    <row r="415" ht="15.75" customHeight="1"/>
-    <row r="416" ht="15.75" customHeight="1"/>
+      <c r="A371" s="3" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="372" ht="15.75" customHeight="1" spans="1:1">
+      <c r="A372" s="3" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="373" ht="15.75" customHeight="1" spans="1:1">
+      <c r="A373" s="3" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="374" ht="15.75" customHeight="1" spans="1:1">
+      <c r="A374" s="3" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="375" ht="15.75" customHeight="1" spans="1:1">
+      <c r="A375" s="3" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="376" ht="15.75" customHeight="1" spans="1:1">
+      <c r="A376" s="3" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="377" ht="15.75" customHeight="1" spans="1:1">
+      <c r="A377" s="3" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="378" ht="15.75" customHeight="1" spans="1:1">
+      <c r="A378" s="3" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="379" ht="15.75" customHeight="1" spans="1:1">
+      <c r="A379" s="3" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="380" ht="15.75" customHeight="1" spans="1:1">
+      <c r="A380" s="3" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="381" ht="15.75" customHeight="1" spans="1:1">
+      <c r="A381" s="3" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="382" ht="15.75" customHeight="1" spans="1:1">
+      <c r="A382" s="3" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="383" ht="15.75" customHeight="1" spans="1:1">
+      <c r="A383" s="3" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="384" ht="15.75" customHeight="1" spans="1:1">
+      <c r="A384" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="385" ht="15.75" customHeight="1" spans="1:1">
+      <c r="A385" s="3" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="386" ht="15.75" customHeight="1" spans="1:1">
+      <c r="A386" s="3" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="387" ht="15.75" customHeight="1" spans="1:1">
+      <c r="A387" s="3" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="388" ht="15.75" customHeight="1" spans="1:1">
+      <c r="A388" s="3" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="389" ht="15.75" customHeight="1" spans="1:1">
+      <c r="A389" s="3" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="390" ht="15.75" customHeight="1" spans="1:1">
+      <c r="A390" s="3" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="391" ht="15.75" customHeight="1" spans="1:1">
+      <c r="A391" s="3" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="392" ht="15.75" customHeight="1" spans="1:1">
+      <c r="A392" s="3" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="393" ht="15.75" customHeight="1" spans="1:1">
+      <c r="A393" s="3" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="394" ht="15.75" customHeight="1" spans="1:1">
+      <c r="A394" s="3" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="395" ht="15.75" customHeight="1" spans="1:1">
+      <c r="A395" s="3" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="396" ht="15.75" customHeight="1" spans="1:1">
+      <c r="A396" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="397" ht="15.75" customHeight="1" spans="1:1">
+      <c r="A397" s="3" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="398" ht="15.75" customHeight="1" spans="1:1">
+      <c r="A398" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="399" ht="15.75" customHeight="1" spans="1:1">
+      <c r="A399" s="3" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="400" ht="15.75" customHeight="1" spans="1:1">
+      <c r="A400" s="3" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="401" ht="15.75" customHeight="1" spans="1:1">
+      <c r="A401" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="402" ht="15.75" customHeight="1" spans="1:1">
+      <c r="A402" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="403" ht="15.75" customHeight="1" spans="1:1">
+      <c r="A403" s="3" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="404" ht="15.75" customHeight="1" spans="1:1">
+      <c r="A404" s="3" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="405" ht="15.75" customHeight="1" spans="1:1">
+      <c r="A405" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="406" ht="15.75" customHeight="1" spans="1:1">
+      <c r="A406" s="3" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="407" ht="15.75" customHeight="1" spans="1:1">
+      <c r="A407" s="3" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="408" ht="15.75" customHeight="1" spans="1:1">
+      <c r="A408" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="409" ht="15.75" customHeight="1" spans="1:1">
+      <c r="A409" s="3" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="410" ht="15.75" customHeight="1" spans="1:1">
+      <c r="A410" s="3" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="411" ht="15.75" customHeight="1" spans="1:1">
+      <c r="A411" s="3" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="412" ht="15.75" customHeight="1" spans="1:1">
+      <c r="A412" s="3" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="413" ht="15.75" customHeight="1" spans="1:1">
+      <c r="A413" s="3" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="414" ht="15.75" customHeight="1" spans="1:1">
+      <c r="A414" s="3" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="415" ht="15.75" customHeight="1" spans="1:1">
+      <c r="A415" s="3" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="416" ht="15.75" customHeight="1" spans="1:1">
+      <c r="A416" s="3" t="s">
+        <v>409</v>
+      </c>
+    </row>
     <row r="417" ht="15.75" customHeight="1"/>
     <row r="418" ht="15.75" customHeight="1"/>
     <row r="419" ht="15.75" customHeight="1"/>
@@ -4538,6 +4847,48 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
+    <row r="1002" ht="15.75" customHeight="1"/>
+    <row r="1003" ht="15.75" customHeight="1"/>
+    <row r="1004" ht="15.75" customHeight="1"/>
+    <row r="1005" ht="15.75" customHeight="1"/>
+    <row r="1006" ht="15.75" customHeight="1"/>
+    <row r="1007" ht="15.75" customHeight="1"/>
+    <row r="1008" ht="15.75" customHeight="1"/>
+    <row r="1009" ht="15.75" customHeight="1"/>
+    <row r="1010" ht="15.75" customHeight="1"/>
+    <row r="1011" ht="15.75" customHeight="1"/>
+    <row r="1012" ht="15.75" customHeight="1"/>
+    <row r="1013" ht="15.75" customHeight="1"/>
+    <row r="1014" ht="15.75" customHeight="1"/>
+    <row r="1015" ht="15.75" customHeight="1"/>
+    <row r="1016" ht="15.75" customHeight="1"/>
+    <row r="1017" ht="15.75" customHeight="1"/>
+    <row r="1018" ht="15.75" customHeight="1"/>
+    <row r="1019" ht="15.75" customHeight="1"/>
+    <row r="1020" ht="15.75" customHeight="1"/>
+    <row r="1021" ht="15.75" customHeight="1"/>
+    <row r="1022" ht="15.75" customHeight="1"/>
+    <row r="1023" ht="15.75" customHeight="1"/>
+    <row r="1024" ht="15.75" customHeight="1"/>
+    <row r="1025" ht="15.75" customHeight="1"/>
+    <row r="1026" ht="15.75" customHeight="1"/>
+    <row r="1027" ht="15.75" customHeight="1"/>
+    <row r="1028" ht="15.75" customHeight="1"/>
+    <row r="1029" ht="15.75" customHeight="1"/>
+    <row r="1030" ht="15.75" customHeight="1"/>
+    <row r="1031" ht="15.75" customHeight="1"/>
+    <row r="1032" ht="15.75" customHeight="1"/>
+    <row r="1033" ht="15.75" customHeight="1"/>
+    <row r="1034" ht="15.75" customHeight="1"/>
+    <row r="1035" ht="15.75" customHeight="1"/>
+    <row r="1036" ht="15.75" customHeight="1"/>
+    <row r="1037" ht="15.75" customHeight="1"/>
+    <row r="1038" ht="15.75" customHeight="1"/>
+    <row r="1039" ht="15.75" customHeight="1"/>
+    <row r="1040" ht="15.75" customHeight="1"/>
+    <row r="1041" ht="15.75" customHeight="1"/>
+    <row r="1042" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -4562,42 +4913,42 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>368</v>
+        <v>410</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1" spans="1:1">
       <c r="A2" s="1" t="s">
-        <v>369</v>
+        <v>411</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>370</v>
+        <v>412</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1" spans="1:1">
       <c r="A4" s="1" t="s">
-        <v>371</v>
+        <v>413</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1" spans="1:1">
       <c r="A5" s="1" t="s">
-        <v>372</v>
+        <v>414</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>373</v>
+        <v>415</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1" spans="1:1">
       <c r="A7" s="1" t="s">
-        <v>374</v>
+        <v>416</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1" spans="1:1">
       <c r="A8" s="1" t="s">
-        <v>375</v>
+        <v>417</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1"/>

</xml_diff>